<commit_message>
Tam Hoan thanh Danh muc nhan vien
</commit_message>
<xml_diff>
--- a/Documents/Bảng phân bố nhiêm vụ.xlsx
+++ b/Documents/Bảng phân bố nhiêm vụ.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>Task</t>
   </si>
@@ -101,6 +101,12 @@
   <si>
     <t>Ok</t>
   </si>
+  <si>
+    <t>Ghi chú</t>
+  </si>
+  <si>
+    <t>Thiếu chức năng Log,  chưa có điều kiện xóa NV</t>
+  </si>
 </sst>
 </file>
 
@@ -175,15 +181,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -194,11 +213,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="22" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3753,415 +3772,450 @@
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="4.5703125" style="3" customWidth="1"/>
     <col min="2" max="2" width="38.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="15.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="25" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="23.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="25.140625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="6" width="23.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="24.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="26.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="49.85546875" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5" t="s">
+      <c r="D1" s="10"/>
+      <c r="E1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5" t="s">
+      <c r="F1" s="10"/>
+      <c r="G1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="5"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="2" t="s">
+      <c r="A2" s="10"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="7" t="s">
         <v>7</v>
       </c>
+      <c r="I2" s="14"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
+      <c r="F3" s="6">
+        <v>44084</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="8"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
+      <c r="A4" s="4">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9" t="s">
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
+      <c r="F4" s="6">
+        <v>44084</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="8"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
+      <c r="A5" s="4">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9" t="s">
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
+      <c r="F5" s="6">
+        <v>44084</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="8"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
+      <c r="A6" s="4">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="8"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
+      <c r="A7" s="4">
         <v>5</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="8"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
+      <c r="A8" s="4">
         <v>6</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="8" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
+      <c r="A9" s="4">
         <v>7</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="8"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
+      <c r="A10" s="4">
         <v>8</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="9"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
+      <c r="A11" s="4">
         <v>9</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="J11" s="6">
-        <f ca="1">NOW()</f>
-        <v>44084.10252083333</v>
-      </c>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
+      <c r="A12" s="4">
         <v>10</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="8">
+      <c r="A13" s="4">
         <v>11</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
+      <c r="A14" s="4">
         <v>12</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="8"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="8">
+      <c r="A15" s="4">
         <v>13</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="8"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
+      <c r="A16" s="4">
         <v>14</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="8"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="8">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
         <v>15</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="8"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="8">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
         <v>16</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="8"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="8">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
         <v>17</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="8"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="8">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
         <v>18</v>
       </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="8"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="8">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
         <v>19</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="8"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="8">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
         <v>20</v>
       </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="8"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="8">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
         <v>21</v>
       </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="8"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="8">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
         <v>22</v>
       </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="8"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="8">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
         <v>23</v>
       </c>
-      <c r="B25" s="3"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="8"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="8">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
         <v>24</v>
       </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="A1:A2"/>
     <mergeCell ref="J11:M13"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="I1:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Them Quan ly nhan vien - Quan Lys lich lam viec
</commit_message>
<xml_diff>
--- a/Documents/Bảng phân bố nhiêm vụ.xlsx
+++ b/Documents/Bảng phân bố nhiêm vụ.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
   <si>
     <t>Task</t>
   </si>
@@ -27,22 +27,10 @@
     <t>Người thực hiện</t>
   </si>
   <si>
-    <t>1stTestLog</t>
-  </si>
-  <si>
-    <t>FixLog</t>
-  </si>
-  <si>
     <t>Thắng</t>
   </si>
   <si>
     <t>Viễn</t>
-  </si>
-  <si>
-    <t>Review</t>
-  </si>
-  <si>
-    <t>Merge time</t>
   </si>
   <si>
     <t>STT</t>
@@ -106,6 +94,33 @@
   </si>
   <si>
     <t>Thiếu chức năng Log,  chưa có điều kiện xóa NV</t>
+  </si>
+  <si>
+    <t>LastUpdate</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>Pause</t>
+  </si>
+  <si>
+    <t>processing..</t>
+  </si>
+  <si>
+    <t>Tích hợp vào sơ đồ phòng</t>
+  </si>
+  <si>
+    <t>Quản lý khách đoàn</t>
+  </si>
+  <si>
+    <t>Quản lý nhân sự</t>
+  </si>
+  <si>
+    <t>Lịch làm việc, chấm công....</t>
   </si>
 </sst>
 </file>
@@ -181,7 +196,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -203,6 +218,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -261,7 +279,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp15.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp16.xml><?xml version="1.0" encoding="utf-8"?>
@@ -269,7 +287,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp17.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp18.xml><?xml version="1.0" encoding="utf-8"?>
@@ -341,7 +359,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp33.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp34.xml><?xml version="1.0" encoding="utf-8"?>
@@ -349,7 +367,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp35.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp36.xml><?xml version="1.0" encoding="utf-8"?>
@@ -409,7 +427,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
@@ -421,7 +439,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3769,10 +3787,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -3783,366 +3801,348 @@
     <col min="4" max="4" width="13.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="25" style="1" customWidth="1"/>
     <col min="6" max="6" width="23.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="24.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="26.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="49.85546875" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="7" width="49.85546875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="13" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10" t="s">
+      <c r="D1" s="11"/>
+      <c r="E1" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="11"/>
+      <c r="G1" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="11"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10" t="s">
+      <c r="D2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="10"/>
-      <c r="I1" s="14" t="s">
-        <v>27</v>
-      </c>
+      <c r="E2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="15"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="14"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F3" s="6">
-        <v>44084</v>
-      </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="8"/>
+        <v>44094</v>
+      </c>
+      <c r="G3" s="8"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F4" s="6">
         <v>44084</v>
       </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="8"/>
+      <c r="G4" s="8"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F5" s="6">
         <v>44084</v>
       </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="8"/>
+      <c r="G5" s="8"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="8"/>
+      <c r="E6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="10">
+        <v>44099</v>
+      </c>
+      <c r="G6" s="8"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="8"/>
+      <c r="E7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="6">
+        <v>44134</v>
+      </c>
+      <c r="G7" s="8"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
+      <c r="E8" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="8" t="s">
-        <v>28</v>
+      <c r="G8" s="8" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="8"/>
+      <c r="G9" s="8"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="9"/>
+      <c r="G10" s="9"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
+      <c r="E11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="6">
+        <v>44134</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="12"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
+      <c r="E12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="6">
+        <v>44134</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="8"/>
+      <c r="G14" s="8"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="8"/>
+      <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="8"/>
+      <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="8"/>
+      <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="8"/>
+      <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="8"/>
+      <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>18</v>
       </c>
-      <c r="B20" s="2"/>
+      <c r="B20" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="8"/>
+      <c r="G20" s="8"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>19</v>
       </c>
-      <c r="B21" s="2"/>
+      <c r="B21" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="8"/>
+      <c r="E21" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" s="6">
+        <v>44134</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>20</v>
       </c>
@@ -4151,11 +4151,9 @@
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="8"/>
+      <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>21</v>
       </c>
@@ -4164,11 +4162,9 @@
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="8"/>
+      <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>22</v>
       </c>
@@ -4177,11 +4173,9 @@
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="8"/>
+      <c r="G24" s="8"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>23</v>
       </c>
@@ -4190,11 +4184,9 @@
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="8"/>
+      <c r="G25" s="8"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>24</v>
       </c>
@@ -4203,19 +4195,16 @@
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="8"/>
+      <c r="G26" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="6">
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="J11:M13"/>
+    <mergeCell ref="H11:K13"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="G1:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Chuan bi them dataloader
</commit_message>
<xml_diff>
--- a/Documents/Bảng phân bố nhiêm vụ.xlsx
+++ b/Documents/Bảng phân bố nhiêm vụ.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
   <si>
     <t>Task</t>
   </si>
@@ -121,6 +121,12 @@
   </si>
   <si>
     <t>Lịch làm việc, chấm công....</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Tích hợp vào sơ đồ phòng,thiếu chuyển phòng, in hóa đơn...</t>
   </si>
 </sst>
 </file>
@@ -3790,7 +3796,7 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -3979,7 +3985,7 @@
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="F11" s="6">
         <v>44134</v>
@@ -4008,7 +4014,7 @@
         <v>44134</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H12" s="13"/>
       <c r="I12" s="13"/>

</xml_diff>